<commit_message>
<develop>:(Web 端)<无>  ShopERP 文档
</commit_message>
<xml_diff>
--- a/CoreShop.Document/CoreShop.xlsx
+++ b/CoreShop.Document/CoreShop.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23063" windowHeight="11244"/>
+    <workbookView windowWidth="20231" windowHeight="9395"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -676,7 +676,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -685,9 +685,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -751,6 +748,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1006,14 +1010,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="13.1111111111111" style="1" customWidth="1"/>
-    <col min="2" max="2" width="62.4444444444444" customWidth="1"/>
-    <col min="3" max="3" width="33" style="1" customWidth="1"/>
+    <col min="2" max="2" width="95.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="22.7777777777778" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19" customHeight="1" spans="1:3">
@@ -1042,7 +1046,7 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">

</xml_diff>